<commit_message>
agregue el test de pdf y corregi un par de cosas de pdf
</commit_message>
<xml_diff>
--- a/IncuttiPanzera_TPPatrones/modulo-exportador/tmp/Datos.xlsx
+++ b/IncuttiPanzera_TPPatrones/modulo-exportador/tmp/Datos.xlsx
@@ -14,6 +14,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
     <t>Lucas</t>
   </si>
   <si>
@@ -21,15 +30,6 @@
   </si>
   <si>
     <t>33</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Apellido</t>
-  </si>
-  <si>
-    <t>Edad</t>
   </si>
 </sst>
 </file>

</xml_diff>